<commit_message>
Expenses Tracker System Fixed Report On Dompdf Breaking
</commit_message>
<xml_diff>
--- a/Storage/template.xlsx
+++ b/Storage/template.xlsx
@@ -19,16 +19,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">EXPENSES TRACKING SYSTEM</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +53,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="26"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,9 +104,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -110,14 +130,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I12:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>